<commit_message>
added SRA required fields
</commit_message>
<xml_diff>
--- a/templates/3ASY04_Genomics/3ASY04_Genomics.xlsx
+++ b/templates/3ASY04_Genomics/3ASY04_Genomics.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/DataManagementPlans/SWATE_templates/templates/3ASY04_Genomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F394F2-5FF8-3141-A3D8-4D7ADF3A4056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA725C6-BC91-F849-B66E-B8AF49FAEEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="-4720" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="3ASY04_Genomics" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <author>Dominik Brilhaus</author>
   </authors>
   <commentList>
-    <comment ref="B23" authorId="0" shapeId="0" xr:uid="{6C002665-3E02-CC4A-B4DE-D8D34CB93E03}">
+    <comment ref="B24" authorId="0" shapeId="0" xr:uid="{6C002665-3E02-CC4A-B4DE-D8D34CB93E03}">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU28" authorId="0" shapeId="0" xr:uid="{29AFF87E-4942-DE4F-B54A-76B81F013AF1}">
+    <comment ref="BA29" authorId="0" shapeId="0" xr:uid="{29AFF87E-4942-DE4F-B54A-76B81F013AF1}">
       <text>
         <r>
           <rPr>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="163">
   <si>
     <t>Source Name</t>
   </si>
@@ -545,6 +545,81 @@
   </si>
   <si>
     <t>Term Accession Number [Read length] (#h; #tNFDI4PSO:0000058)</t>
+  </si>
+  <si>
+    <t>ER instruction</t>
+  </si>
+  <si>
+    <t>Parameter [BioSample Accession Number]</t>
+  </si>
+  <si>
+    <t>Term Source REF [BioSample Accession Number] (#h; #tNFDI4PSO:0000078)</t>
+  </si>
+  <si>
+    <t>Term Accession Number [BioSample Accession Number] (#h; #tNFDI4PSO:0000078)</t>
+  </si>
+  <si>
+    <t>biosample_accession</t>
+  </si>
+  <si>
+    <t>BioSample accession. Typically of the form SAMN[number]. NOT SUB[number]!</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>cv</t>
+  </si>
+  <si>
+    <t>library_strategy</t>
+  </si>
+  <si>
+    <t>Parameter [Library source]</t>
+  </si>
+  <si>
+    <t>Term Source REF [Library source] (#h; #tNFDI4PSO:0000055)</t>
+  </si>
+  <si>
+    <t>Term Accession Number [Library source] (#h; #tNFDI4PSO:0000055)</t>
+  </si>
+  <si>
+    <t>library_source</t>
+  </si>
+  <si>
+    <t>library_selection</t>
+  </si>
+  <si>
+    <t>library_layout</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>GENOMIC</t>
+  </si>
+  <si>
+    <t>TRANSCRIPTOMIC</t>
+  </si>
+  <si>
+    <t>METAGENOMIC</t>
+  </si>
+  <si>
+    <t>METATRANSCRIPTOMIC</t>
+  </si>
+  <si>
+    <t>SYNTHETIC</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>instrument_model</t>
+  </si>
+  <si>
+    <t>filetype</t>
+  </si>
+  <si>
+    <t>filename</t>
   </si>
 </sst>
 </file>
@@ -742,7 +817,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -819,15 +894,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -845,7 +915,13 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{DFD47CC1-D918-4340-9505-CC1F645AC6D8}"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="36">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -978,63 +1054,69 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{644C39E7-36F0-9A4B-B432-FC158C4EAA9E}" name="annotationTable2" displayName="annotationTable2" ref="C2:BD3" totalsRowShown="0">
-  <autoFilter ref="C2:BD3" xr:uid="{3BC338A9-04C5-5343-BA22-34CA5045E92A}"/>
-  <tableColumns count="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{644C39E7-36F0-9A4B-B432-FC158C4EAA9E}" name="annotationTable2" displayName="annotationTable2" ref="C2:BJ3" totalsRowShown="0">
+  <autoFilter ref="C2:BJ3" xr:uid="{3BC338A9-04C5-5343-BA22-34CA5045E92A}"/>
+  <tableColumns count="60">
     <tableColumn id="1" xr3:uid="{9ACF2691-D990-5D41-9C6B-275BFA06B6B8}" name="Source Name"/>
     <tableColumn id="2" xr3:uid="{B871C6EF-90A3-1D4E-A537-D8FF5106BDBF}" name="Sample Name"/>
-    <tableColumn id="3" xr3:uid="{94199463-8351-514E-9EAD-DFF200FA0E38}" name="Parameter [Library strategy]" dataDxfId="33"/>
+    <tableColumn id="55" xr3:uid="{E152CF2F-14BD-FF4C-9C84-85F8515AC341}" name="Parameter [BioSample Accession Number]" dataDxfId="1"/>
+    <tableColumn id="56" xr3:uid="{5C167EDB-45C2-D641-BAB8-BFE8DEACCE68}" name="Term Source REF [BioSample Accession Number] (#h; #tNFDI4PSO:0000078)"/>
+    <tableColumn id="57" xr3:uid="{198AE359-A133-8642-8044-8F89BCD37815}" name="Term Accession Number [BioSample Accession Number] (#h; #tNFDI4PSO:0000078)"/>
+    <tableColumn id="3" xr3:uid="{94199463-8351-514E-9EAD-DFF200FA0E38}" name="Parameter [Library strategy]" dataDxfId="35"/>
     <tableColumn id="4" xr3:uid="{B1496354-2C5D-1C48-B0C5-B2D186BB2C34}" name="Term Source REF [Library strategy] (#h; #tNFDI4PSO:0000035)"/>
     <tableColumn id="5" xr3:uid="{99D60052-24DF-8C41-A74E-AA5E1DF3D60B}" name="Term Accession Number [Library strategy] (#h; #tNFDI4PSO:0000035)"/>
-    <tableColumn id="6" xr3:uid="{FC5523AE-20D6-9146-AE4D-5A54F4869A9D}" name="Parameter [Library Selection]" dataDxfId="32"/>
+    <tableColumn id="58" xr3:uid="{E306261F-9878-C141-9481-B9C05D4D26C7}" name="Parameter [Library source]" dataDxfId="0"/>
+    <tableColumn id="59" xr3:uid="{DEDBC27C-F0CB-2B43-963C-A10B6935E9C8}" name="Term Source REF [Library source] (#h; #tNFDI4PSO:0000055)"/>
+    <tableColumn id="60" xr3:uid="{977337CB-48A6-0D43-8CDE-CDDAA9D24F19}" name="Term Accession Number [Library source] (#h; #tNFDI4PSO:0000055)"/>
+    <tableColumn id="6" xr3:uid="{FC5523AE-20D6-9146-AE4D-5A54F4869A9D}" name="Parameter [Library Selection]" dataDxfId="34"/>
     <tableColumn id="7" xr3:uid="{39DA5E12-4B2B-8E43-A47E-CEF96F39EFD4}" name="Term Source REF [Library Selection] (#h; #tNFDI4PSO:0000036)"/>
     <tableColumn id="8" xr3:uid="{B3C8EAFE-44F7-4247-B18F-EAD4B194CFE9}" name="Term Accession Number [Library Selection] (#h; #tNFDI4PSO:0000036)"/>
-    <tableColumn id="9" xr3:uid="{E47A58FD-232F-4440-8623-8F863EBE7722}" name="Parameter [Library layout]" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{E47A58FD-232F-4440-8623-8F863EBE7722}" name="Parameter [Library layout]" dataDxfId="33"/>
     <tableColumn id="10" xr3:uid="{7F27F67A-0619-9744-B635-28EA2E1EE2CA}" name="Term Source REF [Library layout] (#h)"/>
     <tableColumn id="11" xr3:uid="{60293747-D5F7-E740-9296-E1E9B0006AC0}" name="Term Accession Number [Library layout] (#h)"/>
-    <tableColumn id="12" xr3:uid="{1243D851-1C3F-494E-A25C-3B8BB8D0926B}" name="Parameter [Library preparation kit]" dataDxfId="30"/>
-    <tableColumn id="13" xr3:uid="{8E3BDAF6-B635-B24A-A064-4E8E9A22A1D8}" name="Term Source REF [Library preparation kit] (#h; #tNFDI4PSO:0000037)" dataDxfId="29"/>
-    <tableColumn id="14" xr3:uid="{E7CA87C9-F1BA-C441-A762-424DF654E451}" name="Term Accession Number [Library preparation kit] (#h; #tNFDI4PSO:0000037)" dataDxfId="28"/>
-    <tableColumn id="15" xr3:uid="{F4CB138B-D50D-AC40-AB47-F9127516E361}" name="Parameter [Library preparation kit version]" dataDxfId="27"/>
-    <tableColumn id="16" xr3:uid="{F10584D2-46CF-5B44-B4D4-435967CF4AFF}" name="Term Source REF [Library preparation kit version] (#h; #tNFDI4PSO:0000038)" dataDxfId="26"/>
-    <tableColumn id="17" xr3:uid="{C597DC15-81F1-C740-B52D-F69FAB2EA5E6}" name="Term Accession Number [Library preparation kit version] (#h; #tNFDI4PSO:0000038)" dataDxfId="25"/>
-    <tableColumn id="24" xr3:uid="{FC369AF1-57DB-7F44-9BF2-58D513DCFBBA}" name="Parameter [Adapter sequence]" dataDxfId="24"/>
-    <tableColumn id="25" xr3:uid="{4DBE9ADE-00E1-BD41-925D-58DFFE98D935}" name="Term Source REF [Adapter sequence] (#h; #tNFDI4PSO:0000039)" dataDxfId="23"/>
-    <tableColumn id="26" xr3:uid="{F4036B72-D4A4-7C48-A2F5-B6E6967B2009}" name="Term Accession Number [Adapter sequence] (#h; #tNFDI4PSO:0000039)" dataDxfId="22"/>
-    <tableColumn id="18" xr3:uid="{B8BC038B-24B7-F44C-9E5C-5AADB6F15EF6}" name="Parameter [Library DNA amount]" dataDxfId="21"/>
-    <tableColumn id="19" xr3:uid="{FAA5AC46-091B-1B4A-8F08-AB5D3CB6C274}" name="Term Source REF [Library DNA amount] (#h; #tNFDI4PSO:0000056)" dataDxfId="20"/>
-    <tableColumn id="20" xr3:uid="{8F26D9DC-7F46-CA4B-BA48-CDF6A0BF5121}" name="Term Accession Number [Library DNA amount] (#h; #tNFDI4PSO:0000056)" dataDxfId="19"/>
-    <tableColumn id="21" xr3:uid="{796DE5A9-6752-CC40-B4AD-4792F28CD560}" name="Unit [microgram] (#h; #tUO:0000023; #u)" dataDxfId="18"/>
-    <tableColumn id="22" xr3:uid="{F83EB5CC-2304-204F-8A15-FED54D25FADF}" name="Term Source REF [microgram] (#h; #tUO:0000023; #u)" dataDxfId="17"/>
-    <tableColumn id="23" xr3:uid="{692186DD-E1B5-7541-B395-D611B789C3E8}" name="Term Accession Number [microgram] (#h; #tUO:0000023; #u)" dataDxfId="16"/>
-    <tableColumn id="36" xr3:uid="{679A3E25-765D-7C45-BDC0-806065B76B55}" name="Parameter [Next generation sequencing platform]" dataDxfId="15"/>
-    <tableColumn id="37" xr3:uid="{33CD3040-A545-7347-BA9B-FC63F2172F49}" name="Term Source REF [Next generation sequencing platform] (#h; #tNFDI4PSO:0000057)" dataDxfId="14"/>
-    <tableColumn id="38" xr3:uid="{4DEFF927-7CBD-524E-9A84-4476DF61CA99}" name="Term Accession Number [Next generation sequencing platform] (#h; #tNFDI4PSO:0000057)" dataDxfId="13"/>
-    <tableColumn id="27" xr3:uid="{24CCEEDB-A0AF-684D-9D6D-7326D9EFB476}" name="Parameter [Next generation sequencing instrument model]" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{1243D851-1C3F-494E-A25C-3B8BB8D0926B}" name="Parameter [Library preparation kit]" dataDxfId="32"/>
+    <tableColumn id="13" xr3:uid="{8E3BDAF6-B635-B24A-A064-4E8E9A22A1D8}" name="Term Source REF [Library preparation kit] (#h; #tNFDI4PSO:0000037)" dataDxfId="31"/>
+    <tableColumn id="14" xr3:uid="{E7CA87C9-F1BA-C441-A762-424DF654E451}" name="Term Accession Number [Library preparation kit] (#h; #tNFDI4PSO:0000037)" dataDxfId="30"/>
+    <tableColumn id="15" xr3:uid="{F4CB138B-D50D-AC40-AB47-F9127516E361}" name="Parameter [Library preparation kit version]" dataDxfId="29"/>
+    <tableColumn id="16" xr3:uid="{F10584D2-46CF-5B44-B4D4-435967CF4AFF}" name="Term Source REF [Library preparation kit version] (#h; #tNFDI4PSO:0000038)" dataDxfId="28"/>
+    <tableColumn id="17" xr3:uid="{C597DC15-81F1-C740-B52D-F69FAB2EA5E6}" name="Term Accession Number [Library preparation kit version] (#h; #tNFDI4PSO:0000038)" dataDxfId="27"/>
+    <tableColumn id="24" xr3:uid="{FC369AF1-57DB-7F44-9BF2-58D513DCFBBA}" name="Parameter [Adapter sequence]" dataDxfId="26"/>
+    <tableColumn id="25" xr3:uid="{4DBE9ADE-00E1-BD41-925D-58DFFE98D935}" name="Term Source REF [Adapter sequence] (#h; #tNFDI4PSO:0000039)" dataDxfId="25"/>
+    <tableColumn id="26" xr3:uid="{F4036B72-D4A4-7C48-A2F5-B6E6967B2009}" name="Term Accession Number [Adapter sequence] (#h; #tNFDI4PSO:0000039)" dataDxfId="24"/>
+    <tableColumn id="18" xr3:uid="{B8BC038B-24B7-F44C-9E5C-5AADB6F15EF6}" name="Parameter [Library DNA amount]" dataDxfId="23"/>
+    <tableColumn id="19" xr3:uid="{FAA5AC46-091B-1B4A-8F08-AB5D3CB6C274}" name="Term Source REF [Library DNA amount] (#h; #tNFDI4PSO:0000056)" dataDxfId="22"/>
+    <tableColumn id="20" xr3:uid="{8F26D9DC-7F46-CA4B-BA48-CDF6A0BF5121}" name="Term Accession Number [Library DNA amount] (#h; #tNFDI4PSO:0000056)" dataDxfId="21"/>
+    <tableColumn id="21" xr3:uid="{796DE5A9-6752-CC40-B4AD-4792F28CD560}" name="Unit [microgram] (#h; #tUO:0000023; #u)" dataDxfId="20"/>
+    <tableColumn id="22" xr3:uid="{F83EB5CC-2304-204F-8A15-FED54D25FADF}" name="Term Source REF [microgram] (#h; #tUO:0000023; #u)" dataDxfId="19"/>
+    <tableColumn id="23" xr3:uid="{692186DD-E1B5-7541-B395-D611B789C3E8}" name="Term Accession Number [microgram] (#h; #tUO:0000023; #u)" dataDxfId="18"/>
+    <tableColumn id="36" xr3:uid="{679A3E25-765D-7C45-BDC0-806065B76B55}" name="Parameter [Next generation sequencing platform]" dataDxfId="17"/>
+    <tableColumn id="37" xr3:uid="{33CD3040-A545-7347-BA9B-FC63F2172F49}" name="Term Source REF [Next generation sequencing platform] (#h; #tNFDI4PSO:0000057)" dataDxfId="16"/>
+    <tableColumn id="38" xr3:uid="{4DEFF927-7CBD-524E-9A84-4476DF61CA99}" name="Term Accession Number [Next generation sequencing platform] (#h; #tNFDI4PSO:0000057)" dataDxfId="15"/>
+    <tableColumn id="27" xr3:uid="{24CCEEDB-A0AF-684D-9D6D-7326D9EFB476}" name="Parameter [Next generation sequencing instrument model]" dataDxfId="14"/>
     <tableColumn id="28" xr3:uid="{2BFF580D-CCA0-0345-B808-5F5A1B3D3896}" name="Term Source REF [Next generation sequencing instrument model] (#h; #tNFDI4PSO:0000040)"/>
     <tableColumn id="29" xr3:uid="{95D5E7F6-2884-B745-BDA8-798418A2BD07}" name="Term Accession Number [Next generation sequencing instrument model] (#h; #tNFDI4PSO:0000040)"/>
-    <tableColumn id="30" xr3:uid="{EA7A7326-1A7C-A846-8FBF-E381D349698F}" name="Parameter [Base-calling Software]" dataDxfId="11"/>
+    <tableColumn id="30" xr3:uid="{EA7A7326-1A7C-A846-8FBF-E381D349698F}" name="Parameter [Base-calling Software]" dataDxfId="13"/>
     <tableColumn id="31" xr3:uid="{7D7B7455-8E82-2B46-9BB8-CA37B80DB468}" name="Term Source REF [Base-calling Software] (#h; #tNFDI4PSO:0000017)"/>
     <tableColumn id="32" xr3:uid="{EBDEFF6F-6B01-C54F-AF17-15C2AF95C7AB}" name="Term Accession Number [Base-calling Software] (#h; #tNFDI4PSO:0000017)"/>
-    <tableColumn id="33" xr3:uid="{440360CA-BD83-A24F-ACCB-F08E4E07B309}" name="Parameter [Base-calling Software Version]" dataDxfId="10"/>
+    <tableColumn id="33" xr3:uid="{440360CA-BD83-A24F-ACCB-F08E4E07B309}" name="Parameter [Base-calling Software Version]" dataDxfId="12"/>
     <tableColumn id="34" xr3:uid="{910E1F5D-888F-094B-B509-1D3E5EAF20B2}" name="Term Source REF [Base-calling Software Version] (#h; #tNFDI4PSO:0000018)"/>
     <tableColumn id="35" xr3:uid="{C3192EE8-6CFD-FA41-B093-05A3AFCD5131}" name="Term Accession Number [Base-calling Software Version] (#h; #tNFDI4PSO:0000018)"/>
-    <tableColumn id="39" xr3:uid="{80C1A8E9-93E0-E447-BD7C-42D79D1FCA97}" name="Parameter [Base-calling Software Parameters]" dataDxfId="9"/>
+    <tableColumn id="39" xr3:uid="{80C1A8E9-93E0-E447-BD7C-42D79D1FCA97}" name="Parameter [Base-calling Software Parameters]" dataDxfId="11"/>
     <tableColumn id="40" xr3:uid="{F919BED9-0D13-0D46-8D95-0BE92F377FAA}" name="Term Source REF [Base-calling Software Parameters] (#h; #tNFDI4PSO:0000019)"/>
     <tableColumn id="41" xr3:uid="{4D29BD77-D990-7043-9498-70A782038238}" name="Term Accession Number [Base-calling Software Parameters] (#h; #tNFDI4PSO:0000019)"/>
-    <tableColumn id="42" xr3:uid="{5DEEB0AA-4BC3-F04E-ADAF-CB6EC27B6F47}" name="Parameter [Library strand]" dataDxfId="8"/>
+    <tableColumn id="42" xr3:uid="{5DEEB0AA-4BC3-F04E-ADAF-CB6EC27B6F47}" name="Parameter [Library strand]" dataDxfId="10"/>
     <tableColumn id="43" xr3:uid="{4A2942EF-C8A7-B447-A2D0-71C6825B7E67}" name="Term Source REF [Library strand] (#h; #tNFDI4PSO:0000020)"/>
     <tableColumn id="44" xr3:uid="{F8E13DAD-A5E8-6043-93D9-AAF673CBB1AE}" name="Term Accession Number [Library strand] (#h; #tNFDI4PSO:0000020)"/>
-    <tableColumn id="52" xr3:uid="{E7E6FEA2-AB70-8C4A-B40C-54EFF896F878}" name="Parameter [Read length]" dataDxfId="7"/>
+    <tableColumn id="52" xr3:uid="{E7E6FEA2-AB70-8C4A-B40C-54EFF896F878}" name="Parameter [Read length]" dataDxfId="9"/>
     <tableColumn id="53" xr3:uid="{AE06E2F0-44B3-8644-966F-608194A23A29}" name="Term Source REF [Read length] (#h; #tNFDI4PSO:0000058)"/>
     <tableColumn id="54" xr3:uid="{D56FE0C5-B6BE-3C4A-A478-9CDAB6B15461}" name="Term Accession Number [Read length] (#h; #tNFDI4PSO:0000058)"/>
-    <tableColumn id="45" xr3:uid="{6485F3EF-9735-B74E-958B-107722DC588D}" name="Data File Name" dataDxfId="6"/>
-    <tableColumn id="46" xr3:uid="{0425BA52-9F21-3C43-9855-4DCF1AB9FDC8}" name="Parameter [Raw data file format]" dataDxfId="5"/>
-    <tableColumn id="47" xr3:uid="{FFB5D601-D1A6-E247-9839-723F644EC700}" name="Term Source REF [Raw data file format] (#h; #tNFDI4PSO:0000021)" dataDxfId="4"/>
-    <tableColumn id="48" xr3:uid="{C692B159-D0C9-534A-A34D-23F9298131E4}" name="Term Accession Number [Raw data file format] (#h; #tNFDI4PSO:0000021)" dataDxfId="3"/>
-    <tableColumn id="49" xr3:uid="{00B39407-5107-5447-86CF-D22F8056A82A}" name="Parameter [Raw data file checksum]" dataDxfId="2"/>
-    <tableColumn id="50" xr3:uid="{4EC9F64B-15B4-AE42-8B72-B0FEA0C2E349}" name="Term Source REF [Raw data file checksum] (#h; #tNFDI4PSO:0000022)" dataDxfId="1"/>
-    <tableColumn id="51" xr3:uid="{F5E8E62E-F8E6-814B-B57F-6C79EC78A7D1}" name="Term Accession Number [Raw data file checksum] (#h; #tNFDI4PSO:0000022)" dataDxfId="0"/>
+    <tableColumn id="45" xr3:uid="{6485F3EF-9735-B74E-958B-107722DC588D}" name="Data File Name" dataDxfId="8"/>
+    <tableColumn id="46" xr3:uid="{0425BA52-9F21-3C43-9855-4DCF1AB9FDC8}" name="Parameter [Raw data file format]" dataDxfId="7"/>
+    <tableColumn id="47" xr3:uid="{FFB5D601-D1A6-E247-9839-723F644EC700}" name="Term Source REF [Raw data file format] (#h; #tNFDI4PSO:0000021)" dataDxfId="6"/>
+    <tableColumn id="48" xr3:uid="{C692B159-D0C9-534A-A34D-23F9298131E4}" name="Term Accession Number [Raw data file format] (#h; #tNFDI4PSO:0000021)" dataDxfId="5"/>
+    <tableColumn id="49" xr3:uid="{00B39407-5107-5447-86CF-D22F8056A82A}" name="Parameter [Raw data file checksum]" dataDxfId="4"/>
+    <tableColumn id="50" xr3:uid="{4EC9F64B-15B4-AE42-8B72-B0FEA0C2E349}" name="Term Source REF [Raw data file checksum] (#h; #tNFDI4PSO:0000022)" dataDxfId="3"/>
+    <tableColumn id="51" xr3:uid="{F5E8E62E-F8E6-814B-B57F-6C79EC78A7D1}" name="Term Accession Number [Raw data file checksum] (#h; #tNFDI4PSO:0000022)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1355,77 +1437,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED1A3CE-FE98-7049-B638-99684531C7F7}">
-  <dimension ref="A1:BD69"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:BJ70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
       <pane xSplit="2" ySplit="21" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
-      <selection pane="bottomRight" activeCell="BH18" sqref="BH18"/>
+      <selection pane="bottomRight" activeCell="BE13" sqref="BE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.5" style="19" customWidth="1"/>
     <col min="2" max="2" width="39.6640625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.83203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.33203125" style="23" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="66.83203125" style="23" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="45.83203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.1640625" style="23" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="68.5" style="23" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="27.5" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="37.1640625" style="23" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="44.6640625" style="23" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="45.83203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="65.6640625" style="23" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="73.1640625" style="23" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="45.83203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="72.83203125" style="23" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="80.33203125" style="23" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="45.83203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="62.83203125" style="23" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="70.33203125" style="23" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="33.5" style="23" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="64" style="23" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="71.6640625" style="23" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="42.1640625" style="23" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="52.83203125" style="23" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="60.5" style="23" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="49.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="80" style="23" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="87.5" style="23" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="58.5" style="23" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="89" style="23" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="96.6640625" style="23" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="47.83203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="64.83203125" style="23" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="72.5" style="23" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="42.1640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="72.5" style="23" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="80" style="23" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="45" style="23" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="75.5" style="23" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="83" style="23" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="27.5" style="23" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="58" style="23" hidden="1" customWidth="1"/>
-    <col min="46" max="46" width="65.6640625" style="23" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="26.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="57" style="23" hidden="1" customWidth="1"/>
-    <col min="49" max="49" width="64.5" style="23" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="35.5" style="23" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="33.5" style="23" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="64" style="23" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="71.6640625" style="23" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="37" style="23" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="67.33203125" style="23" hidden="1" customWidth="1"/>
-    <col min="56" max="56" width="74.83203125" style="23" hidden="1" customWidth="1"/>
-    <col min="57" max="16384" width="10.83203125" style="23"/>
+    <col min="3" max="3" width="15" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.5" style="23" customWidth="1"/>
+    <col min="6" max="6" width="68.5" style="23" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="75.1640625" style="23" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="44.1640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="56.33203125" style="23" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="62.83203125" style="23" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="44.1640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="55" style="23" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="61.83203125" style="23" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="29.1640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="57.33203125" style="23" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="64.1640625" style="23" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="44.1640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35.33203125" style="23" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="41.6640625" style="23" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="44.1640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="62.1640625" style="23" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="68.83203125" style="23" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="44.1640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="68.83203125" style="23" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="75.5" style="23" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="30.5" style="23" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="58.6640625" style="23" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="65.5" style="23" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="32" style="23" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="60.33203125" style="23" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="67" style="23" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="38.83203125" style="23" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="49.33203125" style="23" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="56" style="23" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="46.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="75" style="23" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="81.6640625" style="23" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="55" style="23" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="83.33203125" style="23" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="90" style="23" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="32.83203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="61.5" style="23" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="67.6640625" style="23" hidden="1" customWidth="1"/>
+    <col min="44" max="44" width="39.83203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="68.33203125" style="23" hidden="1" customWidth="1"/>
+    <col min="46" max="46" width="74.83203125" style="23" hidden="1" customWidth="1"/>
+    <col min="47" max="47" width="43.1640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="71.83203125" style="23" hidden="1" customWidth="1"/>
+    <col min="49" max="49" width="78" style="23" hidden="1" customWidth="1"/>
+    <col min="50" max="50" width="26.5" style="23" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="54.6640625" style="23" hidden="1" customWidth="1"/>
+    <col min="52" max="52" width="61.33203125" style="23" hidden="1" customWidth="1"/>
+    <col min="53" max="53" width="35" style="23" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="53" style="23" hidden="1" customWidth="1"/>
+    <col min="55" max="55" width="60" style="23" hidden="1" customWidth="1"/>
+    <col min="56" max="56" width="16.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="31.83203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="60.6640625" style="23" hidden="1" customWidth="1"/>
+    <col min="59" max="59" width="66.83203125" style="23" hidden="1" customWidth="1"/>
+    <col min="60" max="60" width="34.5" style="23" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="63.1640625" style="23" hidden="1" customWidth="1"/>
+    <col min="62" max="62" width="69.33203125" style="23" hidden="1" customWidth="1"/>
+    <col min="63" max="16384" width="10.83203125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>45</v>
       </c>
@@ -1483,9 +1572,15 @@
       <c r="BA1" s="4"/>
       <c r="BB1" s="4"/>
       <c r="BC1" s="4"/>
-      <c r="BD1" s="2"/>
-    </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BD1" s="4"/>
+      <c r="BE1" s="4"/>
+      <c r="BF1" s="4"/>
+      <c r="BG1" s="4"/>
+      <c r="BH1" s="4"/>
+      <c r="BI1" s="4"/>
+      <c r="BJ1" s="2"/>
+    </row>
+    <row r="2" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>45</v>
       </c>
@@ -1497,163 +1592,181 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
+        <v>147</v>
+      </c>
+      <c r="L2" t="s">
+        <v>148</v>
+      </c>
+      <c r="M2" t="s">
+        <v>149</v>
+      </c>
+      <c r="N2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="O2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="P2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" t="s">
+      <c r="Q2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" t="s">
+      <c r="R2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" t="s">
+      <c r="S2" t="s">
         <v>10</v>
       </c>
-      <c r="N2" t="s">
+      <c r="T2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" t="s">
+      <c r="U2" t="s">
         <v>12</v>
       </c>
-      <c r="P2" t="s">
+      <c r="V2" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="W2" t="s">
         <v>14</v>
       </c>
-      <c r="R2" t="s">
+      <c r="X2" t="s">
         <v>15</v>
       </c>
-      <c r="S2" t="s">
+      <c r="Y2" t="s">
         <v>16</v>
       </c>
-      <c r="T2" t="s">
+      <c r="Z2" t="s">
         <v>17</v>
       </c>
-      <c r="U2" t="s">
+      <c r="AA2" t="s">
         <v>18</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AB2" t="s">
         <v>19</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AC2" t="s">
         <v>129</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AD2" t="s">
         <v>130</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AE2" t="s">
         <v>131</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AF2" t="s">
         <v>42</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AG2" t="s">
         <v>43</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AH2" t="s">
         <v>44</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AI2" t="s">
         <v>132</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AJ2" t="s">
         <v>133</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AK2" t="s">
         <v>134</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AL2" t="s">
         <v>20</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AM2" t="s">
         <v>21</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AN2" t="s">
         <v>22</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AO2" t="s">
         <v>23</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AP2" t="s">
         <v>24</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AQ2" t="s">
         <v>25</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AR2" t="s">
         <v>26</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AS2" t="s">
         <v>27</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AT2" t="s">
         <v>28</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AU2" t="s">
         <v>29</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AV2" t="s">
         <v>30</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AW2" t="s">
         <v>31</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AX2" t="s">
         <v>32</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AY2" t="s">
         <v>33</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AZ2" t="s">
         <v>34</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="BA2" t="s">
         <v>135</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="BB2" t="s">
         <v>136</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="BC2" t="s">
         <v>137</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="BD2" t="s">
         <v>35</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="BE2" t="s">
         <v>36</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BF2" t="s">
         <v>37</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BG2" t="s">
         <v>38</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BH2" t="s">
         <v>39</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BI2" t="s">
         <v>40</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BJ2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>45</v>
       </c>
@@ -1673,26 +1786,26 @@
       <c r="O3"/>
       <c r="P3"/>
       <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
+      <c r="R3"/>
+      <c r="S3"/>
       <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="48"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3" s="3"/>
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
-      <c r="AC3" s="3"/>
+      <c r="AC3" s="45"/>
       <c r="AD3" s="3"/>
       <c r="AE3" s="3"/>
       <c r="AF3" s="3"/>
-      <c r="AG3"/>
-      <c r="AH3"/>
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="3"/>
       <c r="AI3" s="3"/>
-      <c r="AJ3"/>
-      <c r="AK3"/>
+      <c r="AJ3" s="3"/>
+      <c r="AK3" s="3"/>
       <c r="AL3" s="3"/>
       <c r="AM3"/>
       <c r="AN3"/>
@@ -1706,14 +1819,20 @@
       <c r="AV3"/>
       <c r="AW3"/>
       <c r="AX3" s="3"/>
-      <c r="AY3" s="3"/>
-      <c r="AZ3" s="3"/>
+      <c r="AY3"/>
+      <c r="AZ3"/>
       <c r="BA3" s="3"/>
-      <c r="BB3" s="3"/>
-      <c r="BC3" s="3"/>
+      <c r="BB3"/>
+      <c r="BC3"/>
       <c r="BD3" s="3"/>
-    </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE3" s="3"/>
+      <c r="BF3" s="3"/>
+      <c r="BG3" s="3"/>
+      <c r="BH3" s="3"/>
+      <c r="BI3" s="3"/>
+      <c r="BJ3" s="3"/>
+    </row>
+    <row r="4" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="24"/>
@@ -1771,125 +1890,135 @@
       <c r="BC4" s="24"/>
       <c r="BD4" s="24"/>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="25"/>
       <c r="D5" s="25"/>
-      <c r="E5" s="28" t="s">
-        <v>62</v>
-      </c>
+      <c r="E5" s="25"/>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
       <c r="H5" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
-      <c r="K5" s="28" t="s">
-        <v>64</v>
+      <c r="K5" s="25" t="s">
+        <v>154</v>
       </c>
       <c r="L5" s="25"/>
       <c r="M5" s="25"/>
       <c r="N5" s="28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O5" s="25"/>
       <c r="P5" s="25"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
+      <c r="Q5" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
       <c r="T5" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="U5" s="28"/>
-      <c r="V5" s="28"/>
+        <v>65</v>
+      </c>
+      <c r="U5" s="25"/>
+      <c r="V5" s="25"/>
       <c r="W5" s="28"/>
       <c r="X5" s="28"/>
       <c r="Y5" s="28"/>
-      <c r="Z5" s="28"/>
+      <c r="Z5" s="28" t="s">
+        <v>66</v>
+      </c>
       <c r="AA5" s="28"/>
       <c r="AB5" s="28"/>
       <c r="AC5" s="28"/>
       <c r="AD5" s="28"/>
       <c r="AE5" s="28"/>
-      <c r="AF5" s="28" t="s">
-        <v>67</v>
-      </c>
+      <c r="AF5" s="28"/>
       <c r="AG5" s="28"/>
       <c r="AH5" s="28"/>
-      <c r="AI5" s="28" t="s">
-        <v>68</v>
-      </c>
+      <c r="AI5" s="28"/>
       <c r="AJ5" s="28"/>
       <c r="AK5" s="28"/>
-      <c r="AL5" s="25">
+      <c r="AL5" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM5" s="28"/>
+      <c r="AN5" s="28"/>
+      <c r="AO5" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP5" s="28"/>
+      <c r="AQ5" s="28"/>
+      <c r="AR5" s="25">
         <v>1.7</v>
-      </c>
-      <c r="AM5" s="25"/>
-      <c r="AN5" s="25"/>
-      <c r="AO5" s="25"/>
-      <c r="AP5" s="25"/>
-      <c r="AQ5" s="25"/>
-      <c r="AR5" s="28" t="s">
-        <v>70</v>
       </c>
       <c r="AS5" s="25"/>
       <c r="AT5" s="25"/>
-      <c r="AU5" s="28"/>
-      <c r="AV5" s="33" t="s">
-        <v>71</v>
-      </c>
+      <c r="AU5" s="25"/>
+      <c r="AV5" s="25"/>
       <c r="AW5" s="25"/>
       <c r="AX5" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="AY5" s="25"/>
+      <c r="AZ5" s="25"/>
+      <c r="BA5" s="28"/>
+      <c r="BB5" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="BC5" s="25"/>
+      <c r="BD5" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="AY5" s="28"/>
-      <c r="AZ5" s="28"/>
-      <c r="BA5" s="28"/>
-      <c r="BB5" s="33"/>
-      <c r="BC5" s="25"/>
-      <c r="BD5" s="25"/>
-    </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE5" s="28"/>
+      <c r="BF5" s="28"/>
+      <c r="BG5" s="28"/>
+      <c r="BH5" s="33"/>
+      <c r="BI5" s="25"/>
+      <c r="BJ5" s="25"/>
+    </row>
+    <row r="6" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
-      <c r="E6" s="28" t="s">
-        <v>72</v>
-      </c>
+      <c r="E6" s="25"/>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
       <c r="H6" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
-      <c r="K6" s="28" t="s">
-        <v>74</v>
+      <c r="K6" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="L6" s="25"/>
       <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
+      <c r="N6" s="28" t="s">
+        <v>73</v>
+      </c>
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
+      <c r="Q6" s="28" t="s">
+        <v>74</v>
+      </c>
       <c r="R6" s="25"/>
       <c r="S6" s="25"/>
-      <c r="T6" s="25" t="s">
-        <v>75</v>
-      </c>
+      <c r="T6" s="25"/>
       <c r="U6" s="25"/>
       <c r="V6" s="25"/>
       <c r="W6" s="25"/>
       <c r="X6" s="25"/>
       <c r="Y6" s="25"/>
-      <c r="Z6" s="25"/>
+      <c r="Z6" s="25" t="s">
+        <v>75</v>
+      </c>
       <c r="AA6" s="25"/>
       <c r="AB6" s="25"/>
       <c r="AC6" s="25"/>
@@ -1907,61 +2036,69 @@
       <c r="AO6" s="25"/>
       <c r="AP6" s="25"/>
       <c r="AQ6" s="25"/>
-      <c r="AR6" s="28" t="s">
-        <v>77</v>
-      </c>
+      <c r="AR6" s="25"/>
       <c r="AS6" s="25"/>
       <c r="AT6" s="25"/>
-      <c r="AU6" s="28"/>
-      <c r="AV6" s="28" t="s">
-        <v>78</v>
-      </c>
+      <c r="AU6" s="25"/>
+      <c r="AV6" s="25"/>
       <c r="AW6" s="25"/>
       <c r="AX6" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="AY6" s="25"/>
+      <c r="AZ6" s="25"/>
+      <c r="BA6" s="28"/>
+      <c r="BB6" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="BC6" s="25"/>
+      <c r="BD6" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="AY6" s="28"/>
-      <c r="AZ6" s="28"/>
-      <c r="BA6" s="28"/>
-      <c r="BB6" s="28"/>
-      <c r="BC6" s="25"/>
-      <c r="BD6" s="25"/>
-    </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE6" s="28"/>
+      <c r="BF6" s="28"/>
+      <c r="BG6" s="28"/>
+      <c r="BH6" s="28"/>
+      <c r="BI6" s="25"/>
+      <c r="BJ6" s="25"/>
+    </row>
+    <row r="7" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
-      <c r="E7" s="28" t="s">
-        <v>79</v>
-      </c>
+      <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
       <c r="H7" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I7" s="25"/>
       <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
+      <c r="K7" s="25" t="s">
+        <v>156</v>
+      </c>
       <c r="L7" s="25"/>
       <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
+      <c r="N7" s="28" t="s">
+        <v>80</v>
+      </c>
       <c r="O7" s="25"/>
       <c r="P7" s="25"/>
       <c r="Q7" s="25"/>
       <c r="R7" s="25"/>
       <c r="S7" s="25"/>
-      <c r="T7" s="25" t="s">
-        <v>81</v>
-      </c>
+      <c r="T7" s="25"/>
       <c r="U7" s="25"/>
       <c r="V7" s="25"/>
       <c r="W7" s="25"/>
       <c r="X7" s="25"/>
       <c r="Y7" s="25"/>
-      <c r="Z7" s="25"/>
+      <c r="Z7" s="25" t="s">
+        <v>81</v>
+      </c>
       <c r="AA7" s="25"/>
       <c r="AB7" s="25"/>
       <c r="AC7" s="25"/>
@@ -1979,23 +2116,29 @@
       <c r="AO7" s="25"/>
       <c r="AP7" s="25"/>
       <c r="AQ7" s="25"/>
-      <c r="AR7" s="28" t="s">
-        <v>82</v>
-      </c>
+      <c r="AR7" s="25"/>
       <c r="AS7" s="25"/>
       <c r="AT7" s="25"/>
-      <c r="AU7" s="28"/>
+      <c r="AU7" s="25"/>
       <c r="AV7" s="25"/>
       <c r="AW7" s="25"/>
-      <c r="AX7" s="25"/>
+      <c r="AX7" s="28" t="s">
+        <v>82</v>
+      </c>
       <c r="AY7" s="25"/>
       <c r="AZ7" s="25"/>
-      <c r="BA7" s="25"/>
+      <c r="BA7" s="28"/>
       <c r="BB7" s="25"/>
       <c r="BC7" s="25"/>
       <c r="BD7" s="25"/>
-    </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE7" s="25"/>
+      <c r="BF7" s="25"/>
+      <c r="BG7" s="25"/>
+      <c r="BH7" s="25"/>
+      <c r="BI7" s="25"/>
+      <c r="BJ7" s="25"/>
+    </row>
+    <row r="8" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>46</v>
       </c>
@@ -2008,7 +2151,9 @@
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
+      <c r="K8" s="25" t="s">
+        <v>157</v>
+      </c>
       <c r="L8" s="25"/>
       <c r="M8" s="25"/>
       <c r="N8" s="25"/>
@@ -2054,8 +2199,14 @@
       <c r="BB8" s="25"/>
       <c r="BC8" s="25"/>
       <c r="BD8" s="25"/>
-    </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE8" s="25"/>
+      <c r="BF8" s="25"/>
+      <c r="BG8" s="25"/>
+      <c r="BH8" s="25"/>
+      <c r="BI8" s="25"/>
+      <c r="BJ8" s="25"/>
+    </row>
+    <row r="9" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>46</v>
       </c>
@@ -2068,7 +2219,9 @@
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
       <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
+      <c r="K9" s="25" t="s">
+        <v>158</v>
+      </c>
       <c r="L9" s="25"/>
       <c r="M9" s="25"/>
       <c r="N9" s="25"/>
@@ -2114,8 +2267,14 @@
       <c r="BB9" s="25"/>
       <c r="BC9" s="25"/>
       <c r="BD9" s="25"/>
-    </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE9" s="25"/>
+      <c r="BF9" s="25"/>
+      <c r="BG9" s="25"/>
+      <c r="BH9" s="25"/>
+      <c r="BI9" s="25"/>
+      <c r="BJ9" s="25"/>
+    </row>
+    <row r="10" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="24"/>
@@ -2172,8 +2331,14 @@
       <c r="BB10" s="24"/>
       <c r="BC10" s="24"/>
       <c r="BD10" s="24"/>
-    </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE10" s="24"/>
+      <c r="BF10" s="24"/>
+      <c r="BG10" s="24"/>
+      <c r="BH10" s="24"/>
+      <c r="BI10" s="24"/>
+      <c r="BJ10" s="24"/>
+    </row>
+    <row r="11" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>47</v>
       </c>
@@ -2182,86 +2347,92 @@
       </c>
       <c r="C11" s="26"/>
       <c r="D11" s="26"/>
-      <c r="E11" s="26" t="s">
-        <v>91</v>
-      </c>
+      <c r="E11" s="26"/>
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
       <c r="H11" s="26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I11" s="26"/>
       <c r="J11" s="26"/>
-      <c r="K11" s="26" t="s">
-        <v>94</v>
-      </c>
+      <c r="K11" s="26"/>
       <c r="L11" s="26"/>
       <c r="M11" s="26"/>
       <c r="N11" s="26" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="O11" s="26"/>
       <c r="P11" s="26"/>
       <c r="Q11" s="26" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="R11" s="26"/>
       <c r="S11" s="26"/>
       <c r="T11" s="26" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="U11" s="26"/>
       <c r="V11" s="26"/>
-      <c r="W11" s="26"/>
+      <c r="W11" s="26" t="s">
+        <v>102</v>
+      </c>
       <c r="X11" s="26"/>
       <c r="Y11" s="26"/>
-      <c r="Z11" s="26"/>
+      <c r="Z11" s="26" t="s">
+        <v>106</v>
+      </c>
       <c r="AA11" s="26"/>
       <c r="AB11" s="26"/>
       <c r="AC11" s="26"/>
       <c r="AD11" s="26"/>
       <c r="AE11" s="26"/>
-      <c r="AF11" s="26" t="s">
-        <v>110</v>
-      </c>
+      <c r="AF11" s="26"/>
       <c r="AG11" s="26"/>
       <c r="AH11" s="26"/>
-      <c r="AI11" s="26" t="s">
-        <v>116</v>
-      </c>
+      <c r="AI11" s="26"/>
       <c r="AJ11" s="26"/>
       <c r="AK11" s="26"/>
       <c r="AL11" s="26" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="AM11" s="26"/>
       <c r="AN11" s="26"/>
       <c r="AO11" s="26" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="AP11" s="26"/>
       <c r="AQ11" s="26"/>
       <c r="AR11" s="26" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AS11" s="26"/>
       <c r="AT11" s="26"/>
-      <c r="AU11" s="26"/>
-      <c r="AV11" s="26" t="s">
-        <v>124</v>
-      </c>
+      <c r="AU11" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV11" s="26"/>
       <c r="AW11" s="26"/>
-      <c r="AX11" s="26"/>
+      <c r="AX11" s="26" t="s">
+        <v>122</v>
+      </c>
       <c r="AY11" s="26"/>
       <c r="AZ11" s="26"/>
       <c r="BA11" s="26"/>
       <c r="BB11" s="26" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="BC11" s="26"/>
       <c r="BD11" s="26"/>
-    </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE11" s="26"/>
+      <c r="BF11" s="26"/>
+      <c r="BG11" s="26"/>
+      <c r="BH11" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="BI11" s="26"/>
+      <c r="BJ11" s="26"/>
+    </row>
+    <row r="12" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>47</v>
       </c>
@@ -2270,86 +2441,92 @@
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
-      <c r="E12" s="27" t="s">
-        <v>83</v>
-      </c>
+      <c r="E12" s="27"/>
       <c r="F12" s="27"/>
       <c r="G12" s="27"/>
       <c r="H12" s="27" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
-      <c r="K12" s="27" t="s">
-        <v>93</v>
-      </c>
+      <c r="K12" s="27"/>
       <c r="L12" s="27"/>
       <c r="M12" s="27"/>
       <c r="N12" s="27" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="O12" s="27"/>
       <c r="P12" s="27"/>
       <c r="Q12" s="27" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="R12" s="27"/>
       <c r="S12" s="27"/>
       <c r="T12" s="27" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="U12" s="27"/>
       <c r="V12" s="27"/>
-      <c r="W12" s="27"/>
+      <c r="W12" s="27" t="s">
+        <v>99</v>
+      </c>
       <c r="X12" s="27"/>
       <c r="Y12" s="27"/>
-      <c r="Z12" s="27"/>
+      <c r="Z12" s="27" t="s">
+        <v>103</v>
+      </c>
       <c r="AA12" s="27"/>
       <c r="AB12" s="27"/>
       <c r="AC12" s="27"/>
       <c r="AD12" s="27"/>
       <c r="AE12" s="27"/>
-      <c r="AF12" s="27" t="s">
-        <v>107</v>
-      </c>
+      <c r="AF12" s="27"/>
       <c r="AG12" s="27"/>
       <c r="AH12" s="27"/>
-      <c r="AI12" s="27" t="s">
-        <v>115</v>
-      </c>
+      <c r="AI12" s="27"/>
       <c r="AJ12" s="27"/>
       <c r="AK12" s="27"/>
       <c r="AL12" s="27" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="AM12" s="27"/>
       <c r="AN12" s="27"/>
       <c r="AO12" s="27" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="AP12" s="27"/>
       <c r="AQ12" s="27"/>
       <c r="AR12" s="27" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="AS12" s="27"/>
       <c r="AT12" s="27"/>
-      <c r="AU12" s="27"/>
-      <c r="AV12" s="27" t="s">
-        <v>123</v>
-      </c>
+      <c r="AU12" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="AV12" s="27"/>
       <c r="AW12" s="27"/>
-      <c r="AX12" s="27"/>
+      <c r="AX12" s="27" t="s">
+        <v>121</v>
+      </c>
       <c r="AY12" s="27"/>
       <c r="AZ12" s="27"/>
       <c r="BA12" s="27"/>
       <c r="BB12" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="BC12" s="27"/>
       <c r="BD12" s="27"/>
-    </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE12" s="27"/>
+      <c r="BF12" s="27"/>
+      <c r="BG12" s="27"/>
+      <c r="BH12" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="BI12" s="27"/>
+      <c r="BJ12" s="27"/>
+    </row>
+    <row r="13" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>47</v>
       </c>
@@ -2410,8 +2587,14 @@
       <c r="BB13" s="28"/>
       <c r="BC13" s="28"/>
       <c r="BD13" s="28"/>
-    </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE13" s="28"/>
+      <c r="BF13" s="28"/>
+      <c r="BG13" s="28"/>
+      <c r="BH13" s="28"/>
+      <c r="BI13" s="28"/>
+      <c r="BJ13" s="28"/>
+    </row>
+    <row r="14" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>47</v>
       </c>
@@ -2420,13 +2603,11 @@
       </c>
       <c r="C14" s="28"/>
       <c r="D14" s="28"/>
-      <c r="E14" s="28" t="s">
-        <v>84</v>
-      </c>
+      <c r="E14" s="28"/>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
       <c r="H14" s="28" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
@@ -2434,43 +2615,45 @@
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
       <c r="N14" s="28" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="O14" s="28"/>
       <c r="P14" s="28"/>
-      <c r="Q14" s="28" t="s">
-        <v>100</v>
-      </c>
+      <c r="Q14" s="28"/>
       <c r="R14" s="28"/>
       <c r="S14" s="28"/>
       <c r="T14" s="28" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="U14" s="28"/>
       <c r="V14" s="28"/>
-      <c r="W14" s="28"/>
+      <c r="W14" s="28" t="s">
+        <v>100</v>
+      </c>
       <c r="X14" s="28"/>
       <c r="Y14" s="28"/>
-      <c r="Z14" s="28"/>
+      <c r="Z14" s="28" t="s">
+        <v>104</v>
+      </c>
       <c r="AA14" s="28"/>
       <c r="AB14" s="28"/>
       <c r="AC14" s="28"/>
       <c r="AD14" s="28"/>
       <c r="AE14" s="28"/>
-      <c r="AF14" s="28" t="s">
-        <v>108</v>
-      </c>
+      <c r="AF14" s="28"/>
       <c r="AG14" s="28"/>
       <c r="AH14" s="28"/>
-      <c r="AI14" s="28" t="s">
-        <v>111</v>
-      </c>
+      <c r="AI14" s="28"/>
       <c r="AJ14" s="28"/>
       <c r="AK14" s="28"/>
-      <c r="AL14" s="28"/>
+      <c r="AL14" s="28" t="s">
+        <v>108</v>
+      </c>
       <c r="AM14" s="28"/>
       <c r="AN14" s="28"/>
-      <c r="AO14" s="28"/>
+      <c r="AO14" s="28" t="s">
+        <v>111</v>
+      </c>
       <c r="AP14" s="28"/>
       <c r="AQ14" s="28"/>
       <c r="AR14" s="28"/>
@@ -2486,8 +2669,14 @@
       <c r="BB14" s="28"/>
       <c r="BC14" s="28"/>
       <c r="BD14" s="28"/>
-    </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE14" s="28"/>
+      <c r="BF14" s="28"/>
+      <c r="BG14" s="28"/>
+      <c r="BH14" s="28"/>
+      <c r="BI14" s="28"/>
+      <c r="BJ14" s="28"/>
+    </row>
+    <row r="15" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>47</v>
       </c>
@@ -2496,13 +2685,11 @@
       </c>
       <c r="C15" s="29"/>
       <c r="D15" s="29"/>
-      <c r="E15" s="34" t="s">
-        <v>85</v>
-      </c>
+      <c r="E15" s="29"/>
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
       <c r="H15" s="34" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I15" s="29"/>
       <c r="J15" s="29"/>
@@ -2510,43 +2697,45 @@
       <c r="L15" s="29"/>
       <c r="M15" s="29"/>
       <c r="N15" s="34" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="O15" s="29"/>
       <c r="P15" s="29"/>
-      <c r="Q15" s="34" t="s">
-        <v>101</v>
-      </c>
+      <c r="Q15" s="29"/>
       <c r="R15" s="29"/>
       <c r="S15" s="29"/>
       <c r="T15" s="34" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="U15" s="29"/>
       <c r="V15" s="29"/>
-      <c r="W15" s="29"/>
+      <c r="W15" s="34" t="s">
+        <v>101</v>
+      </c>
       <c r="X15" s="29"/>
       <c r="Y15" s="29"/>
-      <c r="Z15" s="29"/>
+      <c r="Z15" s="34" t="s">
+        <v>105</v>
+      </c>
       <c r="AA15" s="29"/>
       <c r="AB15" s="29"/>
       <c r="AC15" s="29"/>
       <c r="AD15" s="29"/>
       <c r="AE15" s="29"/>
-      <c r="AF15" s="29" t="s">
-        <v>109</v>
-      </c>
+      <c r="AF15" s="29"/>
       <c r="AG15" s="29"/>
       <c r="AH15" s="29"/>
-      <c r="AI15" s="34" t="s">
-        <v>112</v>
-      </c>
+      <c r="AI15" s="29"/>
       <c r="AJ15" s="29"/>
       <c r="AK15" s="29"/>
-      <c r="AL15" s="29"/>
+      <c r="AL15" s="29" t="s">
+        <v>109</v>
+      </c>
       <c r="AM15" s="29"/>
       <c r="AN15" s="29"/>
-      <c r="AO15" s="29"/>
+      <c r="AO15" s="34" t="s">
+        <v>112</v>
+      </c>
       <c r="AP15" s="29"/>
       <c r="AQ15" s="29"/>
       <c r="AR15" s="29"/>
@@ -2562,8 +2751,14 @@
       <c r="BB15" s="29"/>
       <c r="BC15" s="29"/>
       <c r="BD15" s="29"/>
-    </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE15" s="29"/>
+      <c r="BF15" s="29"/>
+      <c r="BG15" s="29"/>
+      <c r="BH15" s="29"/>
+      <c r="BI15" s="29"/>
+      <c r="BJ15" s="29"/>
+    </row>
+    <row r="16" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>47</v>
       </c>
@@ -2572,9 +2767,7 @@
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="30"/>
-      <c r="E16" s="30" t="s">
-        <v>86</v>
-      </c>
+      <c r="E16" s="30"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
       <c r="H16" s="30" t="s">
@@ -2585,7 +2778,9 @@
       <c r="K16" s="30"/>
       <c r="L16" s="30"/>
       <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
+      <c r="N16" s="30" t="s">
+        <v>86</v>
+      </c>
       <c r="O16" s="30"/>
       <c r="P16" s="30"/>
       <c r="Q16" s="30"/>
@@ -2606,15 +2801,15 @@
       <c r="AF16" s="30"/>
       <c r="AG16" s="30"/>
       <c r="AH16" s="30"/>
-      <c r="AI16" s="30" t="s">
-        <v>86</v>
-      </c>
+      <c r="AI16" s="30"/>
       <c r="AJ16" s="30"/>
       <c r="AK16" s="30"/>
       <c r="AL16" s="30"/>
       <c r="AM16" s="30"/>
       <c r="AN16" s="30"/>
-      <c r="AO16" s="30"/>
+      <c r="AO16" s="30" t="s">
+        <v>86</v>
+      </c>
       <c r="AP16" s="30"/>
       <c r="AQ16" s="30"/>
       <c r="AR16" s="30"/>
@@ -2627,13 +2822,19 @@
       <c r="AY16" s="30"/>
       <c r="AZ16" s="30"/>
       <c r="BA16" s="30"/>
-      <c r="BB16" s="30" t="s">
-        <v>127</v>
-      </c>
+      <c r="BB16" s="30"/>
       <c r="BC16" s="30"/>
       <c r="BD16" s="30"/>
-    </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE16" s="30"/>
+      <c r="BF16" s="30"/>
+      <c r="BG16" s="30"/>
+      <c r="BH16" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="BI16" s="30"/>
+      <c r="BJ16" s="30"/>
+    </row>
+    <row r="17" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>47</v>
       </c>
@@ -2651,15 +2852,15 @@
       <c r="K17" s="28"/>
       <c r="L17" s="28"/>
       <c r="M17" s="28"/>
-      <c r="N17" s="35" t="s">
-        <v>92</v>
-      </c>
+      <c r="N17" s="28"/>
       <c r="O17" s="28"/>
       <c r="P17" s="28"/>
       <c r="Q17" s="28"/>
       <c r="R17" s="28"/>
       <c r="S17" s="28"/>
-      <c r="T17" s="28"/>
+      <c r="T17" s="35" t="s">
+        <v>92</v>
+      </c>
       <c r="U17" s="28"/>
       <c r="V17" s="28"/>
       <c r="W17" s="28"/>
@@ -2674,15 +2875,15 @@
       <c r="AF17" s="28"/>
       <c r="AG17" s="28"/>
       <c r="AH17" s="28"/>
-      <c r="AI17" s="35" t="s">
-        <v>113</v>
-      </c>
+      <c r="AI17" s="28"/>
       <c r="AJ17" s="28"/>
       <c r="AK17" s="28"/>
       <c r="AL17" s="28"/>
       <c r="AM17" s="28"/>
       <c r="AN17" s="28"/>
-      <c r="AO17" s="28"/>
+      <c r="AO17" s="35" t="s">
+        <v>113</v>
+      </c>
       <c r="AP17" s="28"/>
       <c r="AQ17" s="28"/>
       <c r="AR17" s="28"/>
@@ -2698,8 +2899,14 @@
       <c r="BB17" s="28"/>
       <c r="BC17" s="28"/>
       <c r="BD17" s="28"/>
-    </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE17" s="28"/>
+      <c r="BF17" s="28"/>
+      <c r="BG17" s="28"/>
+      <c r="BH17" s="28"/>
+      <c r="BI17" s="28"/>
+      <c r="BJ17" s="28"/>
+    </row>
+    <row r="18" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>47</v>
       </c>
@@ -2738,15 +2945,15 @@
       <c r="AF18" s="28"/>
       <c r="AG18" s="28"/>
       <c r="AH18" s="28"/>
-      <c r="AI18" s="28" t="s">
-        <v>114</v>
-      </c>
+      <c r="AI18" s="28"/>
       <c r="AJ18" s="28"/>
       <c r="AK18" s="28"/>
       <c r="AL18" s="28"/>
       <c r="AM18" s="28"/>
       <c r="AN18" s="28"/>
-      <c r="AO18" s="28"/>
+      <c r="AO18" s="28" t="s">
+        <v>114</v>
+      </c>
       <c r="AP18" s="28"/>
       <c r="AQ18" s="28"/>
       <c r="AR18" s="28"/>
@@ -2762,8 +2969,14 @@
       <c r="BB18" s="28"/>
       <c r="BC18" s="28"/>
       <c r="BD18" s="28"/>
-    </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE18" s="28"/>
+      <c r="BF18" s="28"/>
+      <c r="BG18" s="28"/>
+      <c r="BH18" s="28"/>
+      <c r="BI18" s="28"/>
+      <c r="BJ18" s="28"/>
+    </row>
+    <row r="19" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>47</v>
       </c>
@@ -2824,8 +3037,14 @@
       <c r="BB19" s="28"/>
       <c r="BC19" s="28"/>
       <c r="BD19" s="28"/>
-    </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE19" s="28"/>
+      <c r="BF19" s="28"/>
+      <c r="BG19" s="28"/>
+      <c r="BH19" s="28"/>
+      <c r="BI19" s="28"/>
+      <c r="BJ19" s="28"/>
+    </row>
+    <row r="20" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A20" s="16"/>
       <c r="B20" s="16"/>
       <c r="C20" s="31"/>
@@ -2882,8 +3101,14 @@
       <c r="BB20" s="31"/>
       <c r="BC20" s="31"/>
       <c r="BD20" s="31"/>
-    </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE20" s="31"/>
+      <c r="BF20" s="31"/>
+      <c r="BG20" s="31"/>
+      <c r="BH20" s="31"/>
+      <c r="BI20" s="31"/>
+      <c r="BJ20" s="31"/>
+    </row>
+    <row r="21" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="31"/>
@@ -2940,8 +3165,14 @@
       <c r="BB21" s="31"/>
       <c r="BC21" s="31"/>
       <c r="BD21" s="31"/>
-    </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BE21" s="31"/>
+      <c r="BF21" s="31"/>
+      <c r="BG21" s="31"/>
+      <c r="BH21" s="31"/>
+      <c r="BI21" s="31"/>
+      <c r="BJ21" s="31"/>
+    </row>
+    <row r="22" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>128</v>
       </c>
@@ -2950,189 +3181,255 @@
       </c>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
-      <c r="E22" s="40"/>
+      <c r="E22" t="s">
+        <v>142</v>
+      </c>
       <c r="F22" s="39"/>
       <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="42"/>
+      <c r="H22" t="s">
+        <v>146</v>
+      </c>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22" t="s">
+        <v>150</v>
+      </c>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22" t="s">
+        <v>151</v>
+      </c>
       <c r="O22" s="39"/>
       <c r="P22" s="39"/>
-      <c r="Q22" s="42"/>
+      <c r="Q22" t="s">
+        <v>152</v>
+      </c>
       <c r="R22" s="39"/>
       <c r="S22" s="39"/>
-      <c r="T22" s="42"/>
+      <c r="T22" s="41"/>
       <c r="U22" s="39"/>
       <c r="V22" s="39"/>
-      <c r="W22" s="39"/>
+      <c r="W22" s="41"/>
       <c r="X22" s="39"/>
       <c r="Y22" s="39"/>
-      <c r="Z22" s="39"/>
+      <c r="Z22" s="41"/>
       <c r="AA22" s="39"/>
       <c r="AB22" s="39"/>
-      <c r="AC22" s="39"/>
-      <c r="AD22" s="39"/>
-      <c r="AE22" s="39"/>
-      <c r="AF22" s="43"/>
-      <c r="AG22" s="39"/>
-      <c r="AH22" s="39"/>
-      <c r="AI22" s="44"/>
-      <c r="AJ22" s="39"/>
-      <c r="AK22" s="39"/>
-      <c r="AL22" s="44"/>
-      <c r="AM22" s="39"/>
-      <c r="AN22" s="39"/>
-      <c r="AO22" s="44"/>
-      <c r="AP22" s="39"/>
-      <c r="AQ22" s="39"/>
-      <c r="AR22" s="44"/>
-      <c r="AS22" s="39"/>
-      <c r="AT22" s="39"/>
-      <c r="AU22" s="43"/>
-      <c r="AV22" s="43"/>
-      <c r="AW22" s="43"/>
-      <c r="AX22" s="39"/>
-      <c r="AY22" s="39"/>
-      <c r="AZ22" s="39"/>
-      <c r="BA22" s="39"/>
-      <c r="BB22" s="43"/>
-      <c r="BC22" s="28"/>
-      <c r="BD22" s="28"/>
-    </row>
-    <row r="23" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="AC22" s="41"/>
+      <c r="AD22" s="41"/>
+      <c r="AE22" s="41"/>
+      <c r="AF22" s="41"/>
+      <c r="AG22" s="41"/>
+      <c r="AH22" s="41"/>
+      <c r="AI22" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="AJ22" s="41"/>
+      <c r="AK22" s="41"/>
+      <c r="AL22" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="AM22" s="41"/>
+      <c r="AN22" s="41"/>
+      <c r="AO22" s="41"/>
+      <c r="AP22" s="41"/>
+      <c r="AQ22" s="41"/>
+      <c r="AR22" s="41"/>
+      <c r="AS22" s="41"/>
+      <c r="AT22" s="41"/>
+      <c r="AU22" s="41"/>
+      <c r="AV22" s="41"/>
+      <c r="AW22" s="41"/>
+      <c r="AX22" s="41"/>
+      <c r="AY22" s="41"/>
+      <c r="AZ22" s="41"/>
+      <c r="BA22" s="41"/>
+      <c r="BB22" s="41"/>
+      <c r="BC22" s="41"/>
+      <c r="BD22" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="BE22" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="BF22" s="41"/>
+      <c r="BG22" s="41"/>
+      <c r="BH22" s="41"/>
+      <c r="BI22" s="28"/>
+      <c r="BJ22" s="28"/>
+    </row>
+    <row r="23" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>128</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>56</v>
+        <v>138</v>
       </c>
       <c r="C23" s="39"/>
       <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
+      <c r="E23" t="s">
+        <v>143</v>
+      </c>
       <c r="F23" s="39"/>
       <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="42"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
       <c r="O23" s="39"/>
       <c r="P23" s="39"/>
-      <c r="Q23" s="42"/>
+      <c r="Q23" s="40"/>
       <c r="R23" s="39"/>
       <c r="S23" s="39"/>
-      <c r="T23" s="42"/>
+      <c r="T23" s="41"/>
       <c r="U23" s="39"/>
       <c r="V23" s="39"/>
-      <c r="W23" s="39"/>
+      <c r="W23" s="41"/>
       <c r="X23" s="39"/>
       <c r="Y23" s="39"/>
-      <c r="Z23" s="39"/>
+      <c r="Z23" s="41"/>
       <c r="AA23" s="39"/>
       <c r="AB23" s="39"/>
-      <c r="AC23" s="39"/>
-      <c r="AD23" s="39"/>
-      <c r="AE23" s="39"/>
-      <c r="AF23" s="39"/>
-      <c r="AG23" s="39"/>
-      <c r="AH23" s="39"/>
-      <c r="AI23" s="39"/>
-      <c r="AJ23" s="39"/>
-      <c r="AK23" s="39"/>
-      <c r="AL23" s="39"/>
-      <c r="AM23" s="39"/>
-      <c r="AN23" s="39"/>
-      <c r="AO23" s="39"/>
-      <c r="AP23" s="39"/>
-      <c r="AQ23" s="39"/>
-      <c r="AR23" s="39"/>
-      <c r="AS23" s="39"/>
-      <c r="AT23" s="39"/>
-      <c r="AU23" s="39"/>
-      <c r="AV23" s="39"/>
-      <c r="AW23" s="39"/>
-      <c r="AX23" s="39"/>
-      <c r="AY23" s="39"/>
-      <c r="AZ23" s="39"/>
-      <c r="BA23" s="39"/>
-      <c r="BB23" s="39"/>
-      <c r="BC23" s="28"/>
-      <c r="BD23" s="28"/>
-    </row>
-    <row r="24" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="AC23" s="41"/>
+      <c r="AD23" s="41"/>
+      <c r="AE23" s="41"/>
+      <c r="AF23" s="41"/>
+      <c r="AG23" s="41"/>
+      <c r="AH23" s="41"/>
+      <c r="AI23" s="41"/>
+      <c r="AJ23" s="41"/>
+      <c r="AK23" s="41"/>
+      <c r="AL23" s="41"/>
+      <c r="AM23" s="41"/>
+      <c r="AN23" s="41"/>
+      <c r="AO23" s="41"/>
+      <c r="AP23" s="41"/>
+      <c r="AQ23" s="41"/>
+      <c r="AR23" s="41"/>
+      <c r="AS23" s="41"/>
+      <c r="AT23" s="41"/>
+      <c r="AU23" s="41"/>
+      <c r="AV23" s="41"/>
+      <c r="AW23" s="41"/>
+      <c r="AX23" s="41"/>
+      <c r="AY23" s="41"/>
+      <c r="AZ23" s="41"/>
+      <c r="BA23" s="41"/>
+      <c r="BB23" s="41"/>
+      <c r="BC23" s="41"/>
+      <c r="BD23" s="41"/>
+      <c r="BE23" s="41"/>
+      <c r="BF23" s="41"/>
+      <c r="BG23" s="41"/>
+      <c r="BH23" s="41"/>
+      <c r="BI23" s="28"/>
+      <c r="BJ23" s="28"/>
+    </row>
+    <row r="24" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>128</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="39"/>
       <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
+      <c r="E24" s="39" t="s">
+        <v>144</v>
+      </c>
       <c r="F24" s="39"/>
       <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
+      <c r="H24" s="39" t="s">
+        <v>145</v>
+      </c>
       <c r="I24" s="39"/>
       <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
+      <c r="K24" s="39" t="s">
+        <v>145</v>
+      </c>
       <c r="L24" s="39"/>
       <c r="M24" s="39"/>
-      <c r="N24" s="39"/>
+      <c r="N24" s="39" t="s">
+        <v>145</v>
+      </c>
       <c r="O24" s="39"/>
       <c r="P24" s="39"/>
-      <c r="Q24" s="39"/>
+      <c r="Q24" s="39" t="s">
+        <v>144</v>
+      </c>
       <c r="R24" s="39"/>
       <c r="S24" s="39"/>
-      <c r="T24" s="39"/>
+      <c r="T24" s="41" t="s">
+        <v>153</v>
+      </c>
       <c r="U24" s="39"/>
       <c r="V24" s="39"/>
-      <c r="W24" s="39"/>
+      <c r="W24" s="41" t="s">
+        <v>153</v>
+      </c>
       <c r="X24" s="39"/>
       <c r="Y24" s="39"/>
-      <c r="Z24" s="39"/>
+      <c r="Z24" s="41" t="s">
+        <v>153</v>
+      </c>
       <c r="AA24" s="39"/>
       <c r="AB24" s="39"/>
-      <c r="AC24" s="39"/>
-      <c r="AD24" s="39"/>
-      <c r="AE24" s="39"/>
-      <c r="AF24" s="39"/>
-      <c r="AG24" s="39"/>
-      <c r="AH24" s="39"/>
-      <c r="AI24" s="39"/>
-      <c r="AJ24" s="39"/>
-      <c r="AK24" s="39"/>
-      <c r="AL24" s="39"/>
-      <c r="AM24" s="39"/>
-      <c r="AN24" s="39"/>
-      <c r="AO24" s="39"/>
-      <c r="AP24" s="39"/>
-      <c r="AQ24" s="39"/>
-      <c r="AR24" s="39"/>
-      <c r="AS24" s="39"/>
-      <c r="AT24" s="39"/>
-      <c r="AU24" s="39"/>
-      <c r="AV24" s="39"/>
-      <c r="AW24" s="39"/>
-      <c r="AX24" s="39"/>
-      <c r="AY24" s="39"/>
-      <c r="AZ24" s="39"/>
-      <c r="BA24" s="39"/>
-      <c r="BB24" s="39"/>
-      <c r="BC24" s="28"/>
-      <c r="BD24" s="28"/>
-    </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="AC24" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="AD24" s="41"/>
+      <c r="AE24" s="41"/>
+      <c r="AF24" s="41"/>
+      <c r="AG24" s="41"/>
+      <c r="AH24" s="41"/>
+      <c r="AI24" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="AJ24" s="41"/>
+      <c r="AK24" s="41"/>
+      <c r="AL24" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM24" s="41"/>
+      <c r="AN24" s="41"/>
+      <c r="AO24" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="AP24" s="41"/>
+      <c r="AQ24" s="41"/>
+      <c r="AR24" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="AS24" s="41"/>
+      <c r="AT24" s="41"/>
+      <c r="AU24" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="AV24" s="41"/>
+      <c r="AW24" s="41"/>
+      <c r="AX24" s="41"/>
+      <c r="AY24" s="41"/>
+      <c r="AZ24" s="41"/>
+      <c r="BA24" s="41"/>
+      <c r="BB24" s="41"/>
+      <c r="BC24" s="41"/>
+      <c r="BD24" s="41"/>
+      <c r="BE24" s="41"/>
+      <c r="BF24" s="41"/>
+      <c r="BG24" s="41"/>
+      <c r="BH24" s="41"/>
+      <c r="BI24" s="28"/>
+      <c r="BJ24" s="28"/>
+    </row>
+    <row r="25" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>128</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" s="39"/>
       <c r="D25" s="39"/>
@@ -3186,15 +3483,21 @@
       <c r="AZ25" s="39"/>
       <c r="BA25" s="39"/>
       <c r="BB25" s="39"/>
-      <c r="BC25" s="28"/>
-      <c r="BD25" s="28"/>
-    </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BC25" s="39"/>
+      <c r="BD25" s="39"/>
+      <c r="BE25" s="39"/>
+      <c r="BF25" s="39"/>
+      <c r="BG25" s="39"/>
+      <c r="BH25" s="39"/>
+      <c r="BI25" s="28"/>
+      <c r="BJ25" s="28"/>
+    </row>
+    <row r="26" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>128</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="39"/>
       <c r="D26" s="39"/>
@@ -3204,7 +3507,7 @@
       <c r="H26" s="39"/>
       <c r="I26" s="39"/>
       <c r="J26" s="39"/>
-      <c r="K26" s="45"/>
+      <c r="K26" s="39"/>
       <c r="L26" s="39"/>
       <c r="M26" s="39"/>
       <c r="N26" s="39"/>
@@ -3237,10 +3540,10 @@
       <c r="AO26" s="39"/>
       <c r="AP26" s="39"/>
       <c r="AQ26" s="39"/>
-      <c r="AR26" s="45"/>
+      <c r="AR26" s="39"/>
       <c r="AS26" s="39"/>
       <c r="AT26" s="39"/>
-      <c r="AU26" s="45"/>
+      <c r="AU26" s="39"/>
       <c r="AV26" s="39"/>
       <c r="AW26" s="39"/>
       <c r="AX26" s="39"/>
@@ -3248,15 +3551,21 @@
       <c r="AZ26" s="39"/>
       <c r="BA26" s="39"/>
       <c r="BB26" s="39"/>
-      <c r="BC26" s="28"/>
-      <c r="BD26" s="28"/>
-    </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="BC26" s="39"/>
+      <c r="BD26" s="39"/>
+      <c r="BE26" s="39"/>
+      <c r="BF26" s="39"/>
+      <c r="BG26" s="39"/>
+      <c r="BH26" s="39"/>
+      <c r="BI26" s="28"/>
+      <c r="BJ26" s="28"/>
+    </row>
+    <row r="27" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>128</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
@@ -3272,7 +3581,7 @@
       <c r="N27" s="39"/>
       <c r="O27" s="39"/>
       <c r="P27" s="39"/>
-      <c r="Q27" s="39"/>
+      <c r="Q27" s="42"/>
       <c r="R27" s="39"/>
       <c r="S27" s="39"/>
       <c r="T27" s="39"/>
@@ -3310,143 +3619,224 @@
       <c r="AZ27" s="39"/>
       <c r="BA27" s="39"/>
       <c r="BB27" s="39"/>
-      <c r="BC27" s="28"/>
-      <c r="BD27" s="28"/>
-    </row>
-    <row r="28" spans="1:56" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="BC27" s="39"/>
+      <c r="BD27" s="39"/>
+      <c r="BE27" s="39"/>
+      <c r="BF27" s="39"/>
+      <c r="BG27" s="39"/>
+      <c r="BH27" s="39"/>
+      <c r="BI27" s="28"/>
+      <c r="BJ27" s="28"/>
+    </row>
+    <row r="28" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39"/>
+      <c r="O28" s="39"/>
+      <c r="P28" s="39"/>
+      <c r="Q28" s="39"/>
+      <c r="R28" s="39"/>
+      <c r="S28" s="39"/>
+      <c r="T28" s="39"/>
+      <c r="U28" s="39"/>
+      <c r="V28" s="39"/>
+      <c r="W28" s="39"/>
+      <c r="X28" s="39"/>
+      <c r="Y28" s="39"/>
+      <c r="Z28" s="39"/>
+      <c r="AA28" s="39"/>
+      <c r="AB28" s="39"/>
+      <c r="AC28" s="39"/>
+      <c r="AD28" s="39"/>
+      <c r="AE28" s="39"/>
+      <c r="AF28" s="39"/>
+      <c r="AG28" s="39"/>
+      <c r="AH28" s="39"/>
+      <c r="AI28" s="39"/>
+      <c r="AJ28" s="39"/>
+      <c r="AK28" s="39"/>
+      <c r="AL28" s="39"/>
+      <c r="AM28" s="39"/>
+      <c r="AN28" s="39"/>
+      <c r="AO28" s="39"/>
+      <c r="AP28" s="39"/>
+      <c r="AQ28" s="39"/>
+      <c r="AR28" s="39"/>
+      <c r="AS28" s="39"/>
+      <c r="AT28" s="39"/>
+      <c r="AU28" s="39"/>
+      <c r="AV28" s="39"/>
+      <c r="AW28" s="39"/>
+      <c r="AX28" s="39"/>
+      <c r="AY28" s="39"/>
+      <c r="AZ28" s="39"/>
+      <c r="BA28" s="39"/>
+      <c r="BB28" s="39"/>
+      <c r="BC28" s="39"/>
+      <c r="BD28" s="39"/>
+      <c r="BE28" s="39"/>
+      <c r="BF28" s="39"/>
+      <c r="BG28" s="39"/>
+      <c r="BH28" s="39"/>
+      <c r="BI28" s="28"/>
+      <c r="BJ28" s="28"/>
+    </row>
+    <row r="29" spans="1:62" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="46"/>
-      <c r="I28" s="46"/>
-      <c r="J28" s="46"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="46"/>
-      <c r="M28" s="46"/>
-      <c r="N28" s="47"/>
-      <c r="O28" s="46"/>
-      <c r="P28" s="46"/>
-      <c r="Q28" s="46"/>
-      <c r="R28" s="46"/>
-      <c r="S28" s="46"/>
-      <c r="T28" s="46"/>
-      <c r="U28" s="46"/>
-      <c r="V28" s="46"/>
-      <c r="W28" s="46"/>
-      <c r="X28" s="46"/>
-      <c r="Y28" s="46"/>
-      <c r="Z28" s="46"/>
-      <c r="AA28" s="46"/>
-      <c r="AB28" s="46"/>
-      <c r="AC28" s="46"/>
-      <c r="AD28" s="46"/>
-      <c r="AE28" s="46"/>
-      <c r="AF28" s="46"/>
-      <c r="AG28" s="46"/>
-      <c r="AH28" s="46"/>
-      <c r="AI28" s="46"/>
-      <c r="AJ28" s="46"/>
-      <c r="AK28" s="46"/>
-      <c r="AL28" s="46"/>
-      <c r="AM28" s="46"/>
-      <c r="AN28" s="46"/>
-      <c r="AO28" s="46"/>
-      <c r="AP28" s="46"/>
-      <c r="AQ28" s="46"/>
-      <c r="AR28" s="46"/>
-      <c r="AS28" s="46"/>
-      <c r="AT28" s="46"/>
-      <c r="AU28" s="45"/>
-      <c r="AV28" s="46"/>
-      <c r="AW28" s="46"/>
-      <c r="AX28" s="46"/>
-      <c r="AY28" s="46"/>
-      <c r="AZ28" s="46"/>
-      <c r="BA28" s="46"/>
-      <c r="BB28" s="46"/>
-      <c r="BC28" s="37"/>
-      <c r="BD28" s="37"/>
-    </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.2">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="32"/>
-      <c r="N29" s="32"/>
-      <c r="O29" s="32"/>
-      <c r="P29" s="32"/>
-      <c r="Q29" s="32"/>
-      <c r="R29" s="32"/>
-      <c r="S29" s="32"/>
-      <c r="T29" s="32"/>
-      <c r="U29" s="32"/>
-      <c r="V29" s="32"/>
-      <c r="W29" s="32"/>
-      <c r="X29" s="32"/>
-      <c r="Y29" s="32"/>
-      <c r="Z29" s="32"/>
-      <c r="AA29" s="32"/>
-      <c r="AB29" s="32"/>
-      <c r="AC29" s="32"/>
-      <c r="AD29" s="32"/>
-      <c r="AE29" s="32"/>
-      <c r="AF29" s="32"/>
-      <c r="AG29" s="32"/>
-      <c r="AH29" s="32"/>
-      <c r="AI29" s="32"/>
-      <c r="AJ29" s="32"/>
-      <c r="AK29" s="32"/>
-      <c r="AL29" s="32"/>
-      <c r="AM29" s="32"/>
-      <c r="AN29" s="32"/>
-      <c r="AO29" s="32"/>
-      <c r="AP29" s="32"/>
-      <c r="AQ29" s="32"/>
-      <c r="AR29" s="32"/>
-      <c r="AS29" s="32"/>
-      <c r="AT29" s="32"/>
-      <c r="AU29" s="32"/>
-      <c r="AV29" s="32"/>
-      <c r="AW29" s="32"/>
-      <c r="AX29" s="32"/>
-      <c r="AY29" s="32"/>
-      <c r="AZ29" s="32"/>
-      <c r="BA29" s="32"/>
-      <c r="BB29" s="32"/>
-      <c r="BC29" s="32"/>
-      <c r="BD29" s="32"/>
-    </row>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.2">
-      <c r="B30" s="20"/>
-    </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="43"/>
+      <c r="P29" s="43"/>
+      <c r="Q29" s="44"/>
+      <c r="R29" s="43"/>
+      <c r="S29" s="43"/>
+      <c r="T29" s="44"/>
+      <c r="U29" s="43"/>
+      <c r="V29" s="43"/>
+      <c r="W29" s="43"/>
+      <c r="X29" s="43"/>
+      <c r="Y29" s="43"/>
+      <c r="Z29" s="43"/>
+      <c r="AA29" s="43"/>
+      <c r="AB29" s="43"/>
+      <c r="AC29" s="43"/>
+      <c r="AD29" s="43"/>
+      <c r="AE29" s="43"/>
+      <c r="AF29" s="43"/>
+      <c r="AG29" s="43"/>
+      <c r="AH29" s="43"/>
+      <c r="AI29" s="43"/>
+      <c r="AJ29" s="43"/>
+      <c r="AK29" s="43"/>
+      <c r="AL29" s="43"/>
+      <c r="AM29" s="43"/>
+      <c r="AN29" s="43"/>
+      <c r="AO29" s="43"/>
+      <c r="AP29" s="43"/>
+      <c r="AQ29" s="43"/>
+      <c r="AR29" s="43"/>
+      <c r="AS29" s="43"/>
+      <c r="AT29" s="43"/>
+      <c r="AU29" s="43"/>
+      <c r="AV29" s="43"/>
+      <c r="AW29" s="43"/>
+      <c r="AX29" s="43"/>
+      <c r="AY29" s="43"/>
+      <c r="AZ29" s="43"/>
+      <c r="BA29" s="43"/>
+      <c r="BB29" s="43"/>
+      <c r="BC29" s="43"/>
+      <c r="BD29" s="43"/>
+      <c r="BE29" s="43"/>
+      <c r="BF29" s="43"/>
+      <c r="BG29" s="43"/>
+      <c r="BH29" s="43"/>
+      <c r="BI29" s="37"/>
+      <c r="BJ29" s="37"/>
+    </row>
+    <row r="30" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="32"/>
+      <c r="Q30" s="32"/>
+      <c r="R30" s="32"/>
+      <c r="S30" s="32"/>
+      <c r="T30" s="32"/>
+      <c r="U30" s="32"/>
+      <c r="V30" s="32"/>
+      <c r="W30" s="32"/>
+      <c r="X30" s="32"/>
+      <c r="Y30" s="32"/>
+      <c r="Z30" s="32"/>
+      <c r="AA30" s="32"/>
+      <c r="AB30" s="32"/>
+      <c r="AC30" s="32"/>
+      <c r="AD30" s="32"/>
+      <c r="AE30" s="32"/>
+      <c r="AF30" s="32"/>
+      <c r="AG30" s="32"/>
+      <c r="AH30" s="32"/>
+      <c r="AI30" s="32"/>
+      <c r="AJ30" s="32"/>
+      <c r="AK30" s="32"/>
+      <c r="AL30" s="32"/>
+      <c r="AM30" s="32"/>
+      <c r="AN30" s="32"/>
+      <c r="AO30" s="32"/>
+      <c r="AP30" s="32"/>
+      <c r="AQ30" s="32"/>
+      <c r="AR30" s="32"/>
+      <c r="AS30" s="32"/>
+      <c r="AT30" s="32"/>
+      <c r="AU30" s="32"/>
+      <c r="AV30" s="32"/>
+      <c r="AW30" s="32"/>
+      <c r="AX30" s="32"/>
+      <c r="AY30" s="32"/>
+      <c r="AZ30" s="32"/>
+      <c r="BA30" s="32"/>
+      <c r="BB30" s="32"/>
+      <c r="BC30" s="32"/>
+      <c r="BD30" s="32"/>
+      <c r="BE30" s="32"/>
+      <c r="BF30" s="32"/>
+      <c r="BG30" s="32"/>
+      <c r="BH30" s="32"/>
+    </row>
+    <row r="31" spans="1:62" x14ac:dyDescent="0.2">
       <c r="B31" s="20"/>
     </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:62" x14ac:dyDescent="0.2">
       <c r="B32" s="20"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="20"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" s="21"/>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="20"/>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B41" s="21"/>
@@ -3523,21 +3913,26 @@
     <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" s="21"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B68" s="22"/>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66" s="21"/>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B69" s="21"/>
+      <c r="B69" s="22"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70" s="21"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E15" r:id="rId1" xr:uid="{121AB7A7-6F7F-F14A-85D5-76293BDEEF72}"/>
-    <hyperlink ref="H15" r:id="rId2" xr:uid="{1B29B5A8-C356-A540-924F-3D4199F43A52}"/>
-    <hyperlink ref="N15" r:id="rId3" xr:uid="{07079257-C442-E440-BEA4-04EE0C7E30DC}"/>
-    <hyperlink ref="Q15" r:id="rId4" xr:uid="{630BD8D1-89DE-4B49-807A-CEB2D7D98DDF}"/>
-    <hyperlink ref="T15" r:id="rId5" xr:uid="{21540447-9E95-E74C-8AAE-FF445045BFA1}"/>
-    <hyperlink ref="AF15" r:id="rId6" xr:uid="{802FB67F-63B8-6F45-A352-CA9DA10EAE18}"/>
-    <hyperlink ref="AI15" r:id="rId7" xr:uid="{0CCD4B95-C043-2842-B7FF-95C38B420646}"/>
+    <hyperlink ref="H15" r:id="rId1" xr:uid="{121AB7A7-6F7F-F14A-85D5-76293BDEEF72}"/>
+    <hyperlink ref="N15" r:id="rId2" xr:uid="{1B29B5A8-C356-A540-924F-3D4199F43A52}"/>
+    <hyperlink ref="T15" r:id="rId3" xr:uid="{07079257-C442-E440-BEA4-04EE0C7E30DC}"/>
+    <hyperlink ref="W15" r:id="rId4" xr:uid="{630BD8D1-89DE-4B49-807A-CEB2D7D98DDF}"/>
+    <hyperlink ref="Z15" r:id="rId5" xr:uid="{21540447-9E95-E74C-8AAE-FF445045BFA1}"/>
+    <hyperlink ref="AL15" r:id="rId6" xr:uid="{802FB67F-63B8-6F45-A352-CA9DA10EAE18}"/>
+    <hyperlink ref="AO15" r:id="rId7" xr:uid="{0CCD4B95-C043-2842-B7FF-95C38B420646}"/>
+    <hyperlink ref="H22" location="'Library and Platform terms'!A2" display="library_strategy (click for details)" xr:uid="{4359DD53-42A0-E145-833D-8D7145FDD287}"/>
+    <hyperlink ref="AI22" location="'Library and Platform terms'!A66" display="platform (click for details)" xr:uid="{8B39E301-37AA-F442-956D-45261F11994C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>